<commit_message>
Change repository status to public
</commit_message>
<xml_diff>
--- a/Estimates/Pathogen10_Marburg_Estimates.xlsx
+++ b/Estimates/Pathogen10_Marburg_Estimates.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Point.estimate</t>
   </si>
@@ -27,9 +27,6 @@
   </si>
   <si>
     <t>SD incubation period (days)</t>
-  </si>
-  <si>
-    <t>95% CI of incubation time (days)</t>
   </si>
 </sst>
 </file>
@@ -120,20 +117,6 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C4" t="n">
-        <v>1.6</v>
-      </c>
-      <c r="D4" t="n">
-        <v>13.8</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>